<commit_message>
redirected users/new to profile/new
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d0fdce2262705b7/University of Ottawa/Winter 2016/CSI 2132 - Databases I/Assignments/Movie_Recommender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qufeichen/Documents/Repos/Movie_Recommender/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="10" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28260" windowHeight="14480" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,12 @@
     <sheet name="studios" sheetId="17" r:id="rId18"/>
     <sheet name="sponsors" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -293,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,22 +324,22 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -346,7 +349,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -354,10 +357,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -365,14 +368,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -380,23 +383,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -734,15 +737,15 @@
       <selection activeCell="K2" sqref="K2:K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="134.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="9" width="11.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="134.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -777,7 +780,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -786,7 +789,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -795,7 +798,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -804,7 +807,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -813,7 +816,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -822,7 +825,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -831,7 +834,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -840,7 +843,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -849,7 +852,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -858,7 +861,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -867,7 +870,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -876,7 +879,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -885,7 +888,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -894,7 +897,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -903,7 +906,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -912,7 +915,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -921,7 +924,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -930,7 +933,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -939,7 +942,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -948,7 +951,7 @@
         <v>INSERT INTO users(user_id, email, password, first_name, last_name, year_born, city, province, country, type_id) VALUES (DEFAULT, '', '', '', '', , '', '', '', );</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -970,15 +973,15 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="111.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="111.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1019,18 +1022,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1063,15 +1064,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>INSERT INTO roles(role_id, character_name) VALUES (DEFAULT, 'Lead');</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>INSERT INTO roles(role_id, character_name) VALUES (DEFAULT, 'Supporting');</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1131,13 +1132,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="64.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="64.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;");"</f>
         <v>INSERT INTO movie_casts(movie_id, actor_id, cast_id) VALUES (, , );</v>
@@ -1170,13 +1171,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO actor_roles("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO actor_roles(actor_id, role_id) VALUES (, );</v>
@@ -1206,13 +1207,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO movie_roles("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO movie_roles(movie_id, role_id) VALUES (, );</v>
@@ -1242,14 +1243,14 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="98.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="98.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1291,13 +1292,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO directs("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO directs(director_id, movie_id) VALUES (, );</v>
@@ -1327,15 +1328,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="69" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1349,7 +1350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1367,17 +1368,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO sponsors("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO sponsors(studio_id, movie_id) VALUES (, );</v>
@@ -1407,15 +1408,15 @@
       <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1432,121 +1433,121 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO profiles("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;") VALUES ("&amp;A2&amp;", '"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"');"</f>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="4" t="str">
         <f t="shared" ref="E3:E21" si="0" xml:space="preserve"> "INSERT INTO profiles("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;") VALUES ("&amp;A3&amp;", '"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"');"</f>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO profiles(user_id, age_range, gender, occupation) VALUES (, '', '', '');</v>
@@ -1565,14 +1566,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1602,17 +1603,17 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="74.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Desktop');</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Laptop');</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Tablet');</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Smartphone');</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Console');</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>INSERT INTO devices(device_id, device_name) VALUES (DEFAULT, 'Smart TV');</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1720,14 +1721,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO devices_used("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO devices_used(user_id, device_id) VALUES (, );</v>
@@ -1757,14 +1758,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Action');</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Adventure');</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1811,7 +1812,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Animation');</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Biography');</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Comedy');</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Crime');</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Documentary');</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Drama');</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Family');</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Fantasy');</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Film-Noir');</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'History');</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Horror');</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Romance');</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Musical');</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Mystery');</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Science Fiction');</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Sport');</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Thriller');</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'War');</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Western');</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Anime');</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Adult');</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Space');</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Political');</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Faith');</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Independent');</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Video Game');</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>INSERT INTO topics(topic_id, genre) VALUES (DEFAULT, 'Novel');</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2148,15 +2149,15 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="145.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="9" width="11.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="145.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2218,7 +2219,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2254,7 +2255,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2290,7 +2291,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2416,7 +2417,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -2434,7 +2435,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2515,7 +2516,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>INSERT INTO movies(movie_id, name, description, date_released, duration, language, subtitles, dubbed, country, age_rating) VALUES (DEFAULT, '', '', '', '', '', '', '', '', '');</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -2564,15 +2565,15 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="87.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="4" width="11.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="87.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO watches("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;", '"&amp;C2&amp;"', "&amp;D2&amp;", '"&amp;E$2&amp;"');"</f>
         <v>INSERT INTO watches(user_id, movie_id, date_watched, user_rating, review) VALUES (, , '', , '');</v>
@@ -2611,14 +2612,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="55.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f xml:space="preserve"> "INSERT INTO movie_topics("&amp;A$1&amp;", "&amp;B$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;");"</f>
         <v>INSERT INTO movie_topics(movie_id, topic_id) VALUES (, );</v>

</xml_diff>

<commit_message>
Fixed all problems with data.sql
Fully functional and ready to be used!
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8880" tabRatio="799" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8880" tabRatio="799" firstSheet="6" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="user_types" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6847" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6847" uniqueCount="1221">
   <si>
     <t>id</t>
   </si>
@@ -3703,6 +3703,9 @@
   </si>
   <si>
     <t>This really isn''t for children….</t>
+  </si>
+  <si>
+    <t>Alfred</t>
   </si>
 </sst>
 </file>
@@ -5409,8 +5412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8893,8 +8896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15858,8 +15861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F113"/>
+    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18364,8 +18367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G144" sqref="G2:G144"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18422,8 +18425,8 @@
         <v>79</v>
       </c>
       <c r="G2" s="6" t="str">
-        <f xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;");"</f>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), Lead, now(), now());</v>
+        <f xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", (SELECT id FROM casting_types WHERE cast_type = '"&amp;D2&amp;"'), "&amp;E2&amp;", "&amp;F2&amp;");"</f>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -18448,8 +18451,8 @@
         <v>79</v>
       </c>
       <c r="G3" s="6" t="str">
-        <f t="shared" ref="G3:G66" si="0" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;");"</f>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Bean'), Support, now(), now());</v>
+        <f t="shared" ref="G3:G66" si="0" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", (SELECT id FROM casting_types WHERE cast_type = '"&amp;D3&amp;"'), "&amp;E3&amp;", "&amp;F3&amp;");"</f>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Bean'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -18475,7 +18478,7 @@
       </c>
       <c r="G4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -18501,7 +18504,7 @@
       </c>
       <c r="G5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -18527,7 +18530,7 @@
       </c>
       <c r="G6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -18553,7 +18556,7 @@
       </c>
       <c r="G7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -18579,7 +18582,7 @@
       </c>
       <c r="G8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -18605,7 +18608,7 @@
       </c>
       <c r="G9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -18631,7 +18634,7 @@
       </c>
       <c r="G10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -18657,7 +18660,7 @@
       </c>
       <c r="G11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Fellowship of the Ring' AND duration = '2:58'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -18683,7 +18686,7 @@
       </c>
       <c r="G12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -18709,7 +18712,7 @@
       </c>
       <c r="G13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -18735,7 +18738,7 @@
       </c>
       <c r="G14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -18761,7 +18764,7 @@
       </c>
       <c r="G15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -18787,7 +18790,7 @@
       </c>
       <c r="G16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -18813,7 +18816,7 @@
       </c>
       <c r="G17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -18839,7 +18842,7 @@
       </c>
       <c r="G18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -18865,7 +18868,7 @@
       </c>
       <c r="G19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -18891,7 +18894,7 @@
       </c>
       <c r="G20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Two Towers' AND duration = '2:59'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -18917,7 +18920,7 @@
       </c>
       <c r="G21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Sean' AND last_name = 'Astin'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -18943,7 +18946,7 @@
       </c>
       <c r="G22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Ian' AND last_name = 'McKellen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -18969,7 +18972,7 @@
       </c>
       <c r="G23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Viggo' AND last_name = 'Mortensen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -18995,7 +18998,7 @@
       </c>
       <c r="G24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Elijah' AND last_name = 'Wood'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -19021,7 +19024,7 @@
       </c>
       <c r="G25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -19047,7 +19050,7 @@
       </c>
       <c r="G26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Cate' AND last_name = 'Blanchett'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -19073,7 +19076,7 @@
       </c>
       <c r="G27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Hugo' AND last_name = 'Weaving'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -19099,7 +19102,7 @@
       </c>
       <c r="G28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Liv' AND last_name = 'Tyler'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -19125,7 +19128,7 @@
       </c>
       <c r="G29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Lord of the Rings: The Return of the King' AND duration = '3:21'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Serkis'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -19151,7 +19154,7 @@
       </c>
       <c r="G30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -19177,7 +19180,7 @@
       </c>
       <c r="G31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Lauren' AND last_name = 'Bacall'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Lauren' AND last_name = 'Bacall'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -19203,7 +19206,7 @@
       </c>
       <c r="G32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Jean' AND last_name = 'Simmons'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Jean' AND last_name = 'Simmons'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -19229,7 +19232,7 @@
       </c>
       <c r="G33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Emily' AND last_name = 'Mortimer'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Howl''s Moving Castle' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Emily' AND last_name = 'Mortimer'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -19255,7 +19258,7 @@
       </c>
       <c r="G34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Ghost' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Patrick' AND last_name = 'Swayze'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Ghost' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Patrick' AND last_name = 'Swayze'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -19281,7 +19284,7 @@
       </c>
       <c r="G35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Ghost' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Demi' AND last_name = 'Moore'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Ghost' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Demi' AND last_name = 'Moore'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -19307,7 +19310,7 @@
       </c>
       <c r="G36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Gena' AND last_name = 'Rowlands'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Gena' AND last_name = 'Rowlands'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -19333,7 +19336,7 @@
       </c>
       <c r="G37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'James' AND last_name = 'Garner'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'James' AND last_name = 'Garner'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -19359,7 +19362,7 @@
       </c>
       <c r="G38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Rachel' AND last_name = 'McAdams'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Rachel' AND last_name = 'McAdams'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -19385,7 +19388,7 @@
       </c>
       <c r="G39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Gosling'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Notebook' AND duration = '2:03'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Gosling'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -19411,7 +19414,7 @@
       </c>
       <c r="G40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Shane' AND last_name = 'West'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Shane' AND last_name = 'West'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -19437,7 +19440,7 @@
       </c>
       <c r="G41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Mandy' AND last_name = 'Moore'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Mandy' AND last_name = 'Moore'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -19463,7 +19466,7 @@
       </c>
       <c r="G42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Peter' AND last_name = 'Coyote'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'A Walk to Remember' AND duration = '1:41'), (SELECT id FROM actors WHERE first_name = 'Peter' AND last_name = 'Coyote'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -19489,7 +19492,7 @@
       </c>
       <c r="G43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Dirty Dancing' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Jennifer' AND last_name = 'Grey'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Dirty Dancing' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Jennifer' AND last_name = 'Grey'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -19515,7 +19518,7 @@
       </c>
       <c r="G44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Dirty Dancing' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Patrick' AND last_name = 'Swayze'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Dirty Dancing' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Patrick' AND last_name = 'Swayze'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -19541,7 +19544,7 @@
       </c>
       <c r="G45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Notting Hill' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Hugh' AND last_name = 'Grant'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Notting Hill' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Hugh' AND last_name = 'Grant'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -19567,7 +19570,7 @@
       </c>
       <c r="G46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Notting Hill' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Notting Hill' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -19593,7 +19596,7 @@
       </c>
       <c r="G47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Pretty Woman' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Pretty Woman' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -19619,7 +19622,7 @@
       </c>
       <c r="G48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Pretty Woman' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Richard' AND last_name = 'Gere'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Pretty Woman' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Richard' AND last_name = 'Gere'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -19645,7 +19648,7 @@
       </c>
       <c r="G49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Say Anything' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'John' AND last_name = 'Cusack'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Say Anything' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'John' AND last_name = 'Cusack'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -19671,7 +19674,7 @@
       </c>
       <c r="G50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Say Anything' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Ione' AND last_name = 'Skye'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Say Anything' AND duration = '1:40'), (SELECT id FROM actors WHERE first_name = 'Ione' AND last_name = 'Skye'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -19697,7 +19700,7 @@
       </c>
       <c r="G51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Leonardo' AND last_name = 'DiCaprio'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Leonardo' AND last_name = 'DiCaprio'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -19723,7 +19726,7 @@
       </c>
       <c r="G52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Kate' AND last_name = 'Winslet'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Kate' AND last_name = 'Winslet'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -19749,7 +19752,7 @@
       </c>
       <c r="G53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Billy' AND last_name = 'Zane'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Titanic' AND duration = '3:14'), (SELECT id FROM actors WHERE first_name = 'Billy' AND last_name = 'Zane'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -19775,7 +19778,7 @@
       </c>
       <c r="G54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'P.S. I Love You' AND duration = '2:06'), (SELECT id FROM actors WHERE first_name = 'Hilary' AND last_name = 'Swank'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'P.S. I Love You' AND duration = '2:06'), (SELECT id FROM actors WHERE first_name = 'Hilary' AND last_name = 'Swank'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -19801,7 +19804,7 @@
       </c>
       <c r="G55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'P.S. I Love You' AND duration = '2:06'), (SELECT id FROM actors WHERE first_name = 'Gerard' AND last_name = 'Butler'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'P.S. I Love You' AND duration = '2:06'), (SELECT id FROM actors WHERE first_name = 'Gerard' AND last_name = 'Butler'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -19827,7 +19830,7 @@
       </c>
       <c r="G56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -19853,7 +19856,7 @@
       </c>
       <c r="G57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Anthony' AND last_name = 'Hopkins'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Anthony' AND last_name = 'Hopkins'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -19879,7 +19882,7 @@
       </c>
       <c r="G58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Aidan' AND last_name = 'Quinn'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Legends of the Fall' AND duration = '2:13'), (SELECT id FROM actors WHERE first_name = 'Aidan' AND last_name = 'Quinn'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -19905,7 +19908,7 @@
       </c>
       <c r="G59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -19931,7 +19934,7 @@
       </c>
       <c r="G60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Eric' AND last_name = 'Bana'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Eric' AND last_name = 'Bana'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -19957,7 +19960,7 @@
       </c>
       <c r="G61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Troy' AND duration = '2:43'), (SELECT id FROM actors WHERE first_name = 'Orlando' AND last_name = 'Bloom'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -19983,7 +19986,7 @@
       </c>
       <c r="G62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Morgan' AND last_name = 'Freeman'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Morgan' AND last_name = 'Freeman'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -20009,7 +20012,7 @@
       </c>
       <c r="G63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -20035,7 +20038,7 @@
       </c>
       <c r="G64" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Kevin' AND last_name = 'Spacey'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Se7en' AND duration = '2:07'), (SELECT id FROM actors WHERE first_name = 'Kevin' AND last_name = 'Spacey'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -20061,7 +20064,7 @@
       </c>
       <c r="G65" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Ziyi' AND last_name = 'Zhang'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Ziyi' AND last_name = 'Zhang'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -20087,7 +20090,7 @@
       </c>
       <c r="G66" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -20112,8 +20115,8 @@
         <v>79</v>
       </c>
       <c r="G67" s="6" t="str">
-        <f t="shared" ref="G67:G130" si="1" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A67&amp;", "&amp;B67&amp;", "&amp;C67&amp;", "&amp;D67&amp;", "&amp;E67&amp;", "&amp;F67&amp;");"</f>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Lau'), Lead, now(), now());</v>
+        <f t="shared" ref="G67:G130" si="1" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A67&amp;", "&amp;B67&amp;", "&amp;C67&amp;", (SELECT id FROM casting_types WHERE cast_type = '"&amp;D67&amp;"'), "&amp;E67&amp;", "&amp;F67&amp;");"</f>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'House of Flying Daggers' AND duration = '1:59'), (SELECT id FROM actors WHERE first_name = 'Andy' AND last_name = 'Lau'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -20139,7 +20142,7 @@
       </c>
       <c r="G68" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Jet' AND last_name = 'Li'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Jet' AND last_name = 'Li'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -20165,7 +20168,7 @@
       </c>
       <c r="G69" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -20191,7 +20194,7 @@
       </c>
       <c r="G70" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Maggie' AND last_name = 'Cheung'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Maggie' AND last_name = 'Cheung'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -20217,7 +20220,7 @@
       </c>
       <c r="G71" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Ziyi' AND last_name = 'Zhang'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Hero' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Ziyi' AND last_name = 'Zhang'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -20243,7 +20246,7 @@
       </c>
       <c r="G72" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -20269,7 +20272,7 @@
       </c>
       <c r="G73" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -20295,7 +20298,7 @@
       </c>
       <c r="G74" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Fengyi' AND last_name = 'Zhang'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff' AND duration = '1:28'), (SELECT id FROM actors WHERE first_name = 'Fengyi' AND last_name = 'Zhang'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -20321,7 +20324,7 @@
       </c>
       <c r="G75" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Tony' AND last_name = 'Chiu Wai Leung'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -20347,7 +20350,7 @@
       </c>
       <c r="G76" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Takeshi' AND last_name = 'Kaneshiro'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -20373,7 +20376,7 @@
       </c>
       <c r="G77" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Fengyi' AND last_name = 'Zhang'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Red Cliff II' AND duration = '1:39'), (SELECT id FROM actors WHERE first_name = 'Fengyi' AND last_name = 'Zhang'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -20399,7 +20402,7 @@
       </c>
       <c r="G78" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Arnold' AND last_name = 'Schwarzenegger'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Arnold' AND last_name = 'Schwarzenegger'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -20425,7 +20428,7 @@
       </c>
       <c r="G79" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Linda' AND last_name = 'Hamilton'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Linda' AND last_name = 'Hamilton'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -20451,7 +20454,7 @@
       </c>
       <c r="G80" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Biehn'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Terminator' AND duration = '1:47'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Biehn'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -20477,7 +20480,7 @@
       </c>
       <c r="G81" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'Sigourney' AND last_name = 'Weaver'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'Sigourney' AND last_name = 'Weaver'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -20503,7 +20506,7 @@
       </c>
       <c r="G82" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Skerritt'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Skerritt'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -20529,7 +20532,7 @@
       </c>
       <c r="G83" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'John' AND last_name = 'Hurt'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Alien' AND duration = '1:57'), (SELECT id FROM actors WHERE first_name = 'John' AND last_name = 'Hurt'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -20555,7 +20558,7 @@
       </c>
       <c r="G84" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Noomi' AND last_name = 'Rapace'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Noomi' AND last_name = 'Rapace'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -20581,7 +20584,7 @@
       </c>
       <c r="G85" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Logan' AND last_name = 'Marshall-Green'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Logan' AND last_name = 'Marshall-Green'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -20607,7 +20610,7 @@
       </c>
       <c r="G86" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Fassbender'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Fassbender'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -20633,7 +20636,7 @@
       </c>
       <c r="G87" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Charlize' AND last_name = 'Theron'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Prometheus' AND duration = '2:04'), (SELECT id FROM actors WHERE first_name = 'Charlize' AND last_name = 'Theron'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -20659,7 +20662,7 @@
       </c>
       <c r="G88" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Dustin' AND last_name = 'Hoffman'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Dustin' AND last_name = 'Hoffman'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -20685,7 +20688,7 @@
       </c>
       <c r="G89" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Sharon' AND last_name = 'Stone'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Sharon' AND last_name = 'Stone'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -20711,7 +20714,7 @@
       </c>
       <c r="G90" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Samuel L.' AND last_name = 'Jackson'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Sphere' AND duration = '2:14'), (SELECT id FROM actors WHERE first_name = 'Samuel L.' AND last_name = 'Jackson'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -20737,7 +20740,7 @@
       </c>
       <c r="G91" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Mark' AND last_name = 'Hamill'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Mark' AND last_name = 'Hamill'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -20763,7 +20766,7 @@
       </c>
       <c r="G92" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Harrison' AND last_name = 'Ford'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Harrison' AND last_name = 'Ford'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -20789,7 +20792,7 @@
       </c>
       <c r="G93" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Carrie' AND last_name = 'Fisher'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Wars: Episode IV – A New Hope' AND duration = '2:01'), (SELECT id FROM actors WHERE first_name = 'Carrie' AND last_name = 'Fisher'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -20815,7 +20818,7 @@
       </c>
       <c r="G94" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -20841,7 +20844,7 @@
       </c>
       <c r="G95" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Steve' AND last_name = 'Carell'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Steve' AND last_name = 'Carell'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -20867,7 +20870,7 @@
       </c>
       <c r="G96" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Gosling'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Gosling'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -20893,7 +20896,7 @@
       </c>
       <c r="G97" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'The Big Short' AND duration = '2:10'), (SELECT id FROM actors WHERE first_name = 'Brad' AND last_name = 'Pitt'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -20919,7 +20922,7 @@
       </c>
       <c r="G98" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '2:16'), (SELECT id FROM actors WHERE first_name = 'Kouji' AND last_name = 'Yakusho'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '2:16'), (SELECT id FROM actors WHERE first_name = 'Kouji' AND last_name = 'Yakusho'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -20945,7 +20948,7 @@
       </c>
       <c r="G99" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '2:16'), (SELECT id FROM actors WHERE first_name = 'Tamiyo' AND last_name = 'Kusakari'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '2:16'), (SELECT id FROM actors WHERE first_name = 'Tamiyo' AND last_name = 'Kusakari'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -20971,7 +20974,7 @@
       </c>
       <c r="G100" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Richard' AND last_name = 'Gere'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Richard' AND last_name = 'Gere'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -20997,7 +21000,7 @@
       </c>
       <c r="G101" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Jennifer' AND last_name = 'Lopez'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Jennifer' AND last_name = 'Lopez'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -21023,7 +21026,7 @@
       </c>
       <c r="G102" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Susan' AND last_name = 'Sarandon'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Shall We Dance?' AND duration = '1:44'), (SELECT id FROM actors WHERE first_name = 'Susan' AND last_name = 'Sarandon'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -21049,7 +21052,7 @@
       </c>
       <c r="G103" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -21075,7 +21078,7 @@
       </c>
       <c r="G104" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Robin' AND last_name = 'Wright'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Robin' AND last_name = 'Wright'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -21101,7 +21104,7 @@
       </c>
       <c r="G105" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Gary' AND last_name = 'Sinise'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Forrest Gump' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Gary' AND last_name = 'Sinise'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -21127,7 +21130,7 @@
       </c>
       <c r="G106" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Hugh' AND last_name = 'Jackman'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Hugh' AND last_name = 'Jackman'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -21153,7 +21156,7 @@
       </c>
       <c r="G107" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Russell' AND last_name = 'Crowe'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Russell' AND last_name = 'Crowe'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -21179,7 +21182,7 @@
       </c>
       <c r="G108" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Anne' AND last_name = 'Hathaway'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Anne' AND last_name = 'Hathaway'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -21205,7 +21208,7 @@
       </c>
       <c r="G109" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Amanda' AND last_name = 'Seyfried'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Amanda' AND last_name = 'Seyfried'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -21231,7 +21234,7 @@
       </c>
       <c r="G110" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Eddie' AND last_name = 'Redmayne'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Les Miserables' AND duration = '2:38'), (SELECT id FROM actors WHERE first_name = 'Eddie' AND last_name = 'Redmayne'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -21257,7 +21260,7 @@
       </c>
       <c r="G111" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Ethan' AND last_name = 'Hawke'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Ethan' AND last_name = 'Hawke'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -21283,7 +21286,7 @@
       </c>
       <c r="G112" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Uma' AND last_name = 'Thurman'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Uma' AND last_name = 'Thurman'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -21309,7 +21312,7 @@
       </c>
       <c r="G113" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Jude' AND last_name = 'Law'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Gattaca' AND duration = '1:46'), (SELECT id FROM actors WHERE first_name = 'Jude' AND last_name = 'Law'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -21335,7 +21338,7 @@
       </c>
       <c r="G114" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -21361,7 +21364,7 @@
       </c>
       <c r="G115" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Julia' AND last_name = 'Roberts'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -21387,7 +21390,7 @@
       </c>
       <c r="G116" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Sarah' AND last_name = 'Mahoney'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Larry Crowne' AND duration = '1:38'), (SELECT id FROM actors WHERE first_name = 'Sarah' AND last_name = 'Mahoney'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -21413,7 +21416,7 @@
       </c>
       <c r="G117" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Up' AND duration = '1:36'), (SELECT id FROM actors WHERE first_name = 'Edward' AND last_name = 'Asner'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Up' AND duration = '1:36'), (SELECT id FROM actors WHERE first_name = 'Edward' AND last_name = 'Asner'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -21439,7 +21442,7 @@
       </c>
       <c r="G118" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Up' AND duration = '1:36'), (SELECT id FROM actors WHERE first_name = 'Jordan' AND last_name = 'Nagai'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Up' AND duration = '1:36'), (SELECT id FROM actors WHERE first_name = 'Jordan' AND last_name = 'Nagai'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -21465,7 +21468,7 @@
       </c>
       <c r="G119" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -21491,7 +21494,7 @@
       </c>
       <c r="G120" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Tim' AND last_name = 'Allen'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Tim' AND last_name = 'Allen'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -21517,7 +21520,7 @@
       </c>
       <c r="G121" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Don' AND last_name = 'Rickles'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Toy Story' AND duration = '1:21'), (SELECT id FROM actors WHERE first_name = 'Don' AND last_name = 'Rickles'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -21543,7 +21546,7 @@
       </c>
       <c r="G122" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Chris' AND last_name = 'Pine'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Chris' AND last_name = 'Pine'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -21569,7 +21572,7 @@
       </c>
       <c r="G123" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Zachary' AND last_name = 'Quinto'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Zachary' AND last_name = 'Quinto'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -21595,7 +21598,7 @@
       </c>
       <c r="G124" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Zoe' AND last_name = 'Saldana'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Zoe' AND last_name = 'Saldana'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -21621,7 +21624,7 @@
       </c>
       <c r="G125" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Benedict' AND last_name = 'Cucumber'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Star Trek: Into Darkness' AND duration = '2:12'), (SELECT id FROM actors WHERE first_name = 'Benedict' AND last_name = 'Cucumber'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -21647,7 +21650,7 @@
       </c>
       <c r="G126" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Christian' AND last_name = 'Bale'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -21673,7 +21676,7 @@
       </c>
       <c r="G127" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Caine'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Caine'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -21699,7 +21702,7 @@
       </c>
       <c r="G128" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Katie' AND last_name = 'Holmes'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Katie' AND last_name = 'Holmes'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -21725,7 +21728,7 @@
       </c>
       <c r="G129" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Liam' AND last_name = 'Neeson'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM actors WHERE first_name = 'Liam' AND last_name = 'Neeson'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -21751,7 +21754,7 @@
       </c>
       <c r="G130" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -21776,8 +21779,8 @@
         <v>79</v>
       </c>
       <c r="G131" s="6" t="str">
-        <f t="shared" ref="G131:G144" si="2" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A131&amp;", "&amp;B131&amp;", "&amp;C131&amp;", "&amp;D131&amp;", "&amp;E131&amp;", "&amp;F131&amp;");"</f>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Mark' AND last_name = 'Rylance'), Support, now(), now());</v>
+        <f t="shared" ref="G131:G144" si="2" xml:space="preserve"> "INSERT INTO movie_casts("&amp;A$1&amp;", "&amp;B$1&amp;", "&amp;C$1&amp;", "&amp;D$1&amp;", "&amp;E$1&amp;", "&amp;F$1&amp;") VALUES ("&amp;A131&amp;", "&amp;B131&amp;", "&amp;C131&amp;", (SELECT id FROM casting_types WHERE cast_type = '"&amp;D131&amp;"'), "&amp;E131&amp;", "&amp;F131&amp;");"</f>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Mark' AND last_name = 'Rylance'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -21803,7 +21806,7 @@
       </c>
       <c r="G132" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Amy' AND last_name = 'Ryan'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Bridge of Spies' AND duration = '2:22'), (SELECT id FROM actors WHERE first_name = 'Amy' AND last_name = 'Ryan'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -21829,7 +21832,7 @@
       </c>
       <c r="G133" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Sam' AND last_name = 'Worthington'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Sam' AND last_name = 'Worthington'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -21855,7 +21858,7 @@
       </c>
       <c r="G134" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Zoe' AND last_name = 'Saldana'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Zoe' AND last_name = 'Saldana'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -21881,7 +21884,7 @@
       </c>
       <c r="G135" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Sigourney' AND last_name = 'Weaver'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Avatar' AND duration = '2:42'), (SELECT id FROM actors WHERE first_name = 'Sigourney' AND last_name = 'Weaver'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -21907,7 +21910,7 @@
       </c>
       <c r="G136" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Reynolds'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Ryan' AND last_name = 'Reynolds'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -21933,7 +21936,7 @@
       </c>
       <c r="G137" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Morena' AND last_name = 'Baccarin'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Morena' AND last_name = 'Baccarin'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -21959,7 +21962,7 @@
       </c>
       <c r="G138" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'T.J.' AND last_name = 'Miller'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'T.J.' AND last_name = 'Miller'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -21985,7 +21988,7 @@
       </c>
       <c r="G139" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Stan' AND last_name = 'Lee'), Cameo, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Deadpool' AND duration = '1:48'), (SELECT id FROM actors WHERE first_name = 'Stan' AND last_name = 'Lee'), (SELECT id FROM casting_types WHERE cast_type = 'Cameo'), now(), now());</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -22011,7 +22014,7 @@
       </c>
       <c r="G140" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Amelie' AND duration = '2:02'), (SELECT id FROM actors WHERE first_name = 'Andrey' AND last_name = 'Tautou'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Amelie' AND duration = '2:02'), (SELECT id FROM actors WHERE first_name = 'Andrey' AND last_name = 'Tautou'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -22037,7 +22040,7 @@
       </c>
       <c r="G141" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Amelie' AND duration = '2:02'), (SELECT id FROM actors WHERE first_name = 'Mathieu' AND last_name = 'Kassovitz'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Amelie' AND duration = '2:02'), (SELECT id FROM actors WHERE first_name = 'Mathieu' AND last_name = 'Kassovitz'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -22063,7 +22066,7 @@
       </c>
       <c r="G142" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Christopher' AND last_name = 'Walken'), Support, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Christopher' AND last_name = 'Walken'), (SELECT id FROM casting_types WHERE cast_type = 'Support'), now(), now());</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -22089,7 +22092,7 @@
       </c>
       <c r="G143" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Leonardo' AND last_name = 'DiCaprio'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Leonardo' AND last_name = 'DiCaprio'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -22115,7 +22118,7 @@
       </c>
       <c r="G144" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), Lead, now(), now());</v>
+        <v>INSERT INTO movie_casts(id, movie_id, actor_id, casting_type_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Catch Me If You Can' AND duration = '2:21'), (SELECT id FROM actors WHERE first_name = 'Tom' AND last_name = 'Hanks'), (SELECT id FROM casting_types WHERE cast_type = 'Lead'), now(), now());</v>
       </c>
     </row>
   </sheetData>
@@ -22127,7 +22130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F126"/>
     </sheetView>
   </sheetViews>
@@ -22135,7 +22138,7 @@
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" customWidth="1"/>
+    <col min="3" max="3" width="59.28515625" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" style="6" customWidth="1"/>
   </cols>
@@ -24631,7 +24634,7 @@
       </c>
       <c r="C109" t="str">
         <f xml:space="preserve"> "(SELECT id FROM roles WHERE character_name = '"&amp;roles!B106&amp;"')"</f>
-        <v>(SELECT id FROM roles WHERE character_name = 'Alfred Ludlow')</v>
+        <v>(SELECT id FROM roles WHERE character_name = 'Alfred')</v>
       </c>
       <c r="D109" t="s">
         <v>79</v>
@@ -24641,7 +24644,7 @@
       </c>
       <c r="F109" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO actor_roles(id, actor_id, role_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Caine'), (SELECT id FROM roles WHERE character_name = 'Alfred Ludlow'), now(), now());</v>
+        <v>INSERT INTO actor_roles(id, actor_id, role_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM actors WHERE first_name = 'Michael' AND last_name = 'Caine'), (SELECT id FROM roles WHERE character_name = 'Alfred'), now(), now());</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -25044,8 +25047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F145" sqref="F2:F145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27985,7 +27988,7 @@
       </c>
       <c r="C128" t="str">
         <f xml:space="preserve"> "(SELECT id FROM roles WHERE character_name = '"&amp;roles!B106&amp;"')"</f>
-        <v>(SELECT id FROM roles WHERE character_name = 'Alfred Ludlow')</v>
+        <v>(SELECT id FROM roles WHERE character_name = 'Alfred')</v>
       </c>
       <c r="D128" t="s">
         <v>79</v>
@@ -27995,7 +27998,7 @@
       </c>
       <c r="F128" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO movie_roles(id, movie_id, role_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM roles WHERE character_name = 'Alfred Ludlow'), now(), now());</v>
+        <v>INSERT INTO movie_roles(id, movie_id, role_id, created_at, updated_at) VALUES (DEFAULT, (SELECT id FROM movies WHERE movie_name = 'Batman Begins' AND duration = '2:20'), (SELECT id FROM roles WHERE character_name = 'Alfred'), now(), now());</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -38701,7 +38704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A98" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E123"/>
     </sheetView>
   </sheetViews>
@@ -40607,7 +40610,7 @@
         <v>72</v>
       </c>
       <c r="B106" t="s">
-        <v>650</v>
+        <v>1220</v>
       </c>
       <c r="C106" t="s">
         <v>79</v>
@@ -40617,7 +40620,7 @@
       </c>
       <c r="E106" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO roles(id, character_name, created_at, updated_at) VALUES (DEFAULT, 'Alfred Ludlow', now(), now());</v>
+        <v>INSERT INTO roles(id, character_name, created_at, updated_at) VALUES (DEFAULT, 'Alfred', now(), now());</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>